<commit_message>
Update Mock 1 test data and reprocess results
Reprocessed Mock 1.xlsx with updated student data and regenerated all JSON data files.

Changes:
- Updated Mock 1.xlsx with corrected student scores
- Reprocessed all test data to reflect changes
- Section thresholds: S1=6.25, S2=0.25, S3=0.25, Essay=12.00 marks

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Results/Mock 1.xlsx
+++ b/Results/Mock 1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\results giver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB2164E-9FCD-43C3-BC93-F77029C1F2D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55BD355-5465-4E2A-B789-CC6A47586B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="164">
   <si>
     <t>ID</t>
   </si>
@@ -232,213 +232,213 @@
     <t>Section1-Q27</t>
   </si>
   <si>
+    <t>Section1-Q5</t>
+  </si>
+  <si>
+    <t>Section2-Q9</t>
+  </si>
+  <si>
+    <t>Section2-Q12</t>
+  </si>
+  <si>
+    <t>Section2-Q3</t>
+  </si>
+  <si>
+    <t>Section3-Q6</t>
+  </si>
+  <si>
+    <t>Section3-Q10</t>
+  </si>
+  <si>
+    <t>Section3-Q7</t>
+  </si>
+  <si>
+    <t>Section1-Q4</t>
+  </si>
+  <si>
+    <t>Section1-Q14</t>
+  </si>
+  <si>
+    <t>Section1-Q10</t>
+  </si>
+  <si>
+    <t>Section2-Q6</t>
+  </si>
+  <si>
+    <t>Section2-Q25</t>
+  </si>
+  <si>
+    <t>Section2-Q13</t>
+  </si>
+  <si>
+    <t>Section3-Q3</t>
+  </si>
+  <si>
+    <t>Section3-Q8</t>
+  </si>
+  <si>
+    <t>Section3-Q4</t>
+  </si>
+  <si>
+    <t>Section1-Q13</t>
+  </si>
+  <si>
+    <t>Section1-Q22</t>
+  </si>
+  <si>
+    <t>Section1-Q11</t>
+  </si>
+  <si>
+    <t>Section2-Q10</t>
+  </si>
+  <si>
+    <t>Section2-Q16</t>
+  </si>
+  <si>
+    <t>Section3-Q2</t>
+  </si>
+  <si>
+    <t>Section1-Q2</t>
+  </si>
+  <si>
+    <t>Section1-Q29</t>
+  </si>
+  <si>
+    <t>Section1-Q20</t>
+  </si>
+  <si>
+    <t>Section2-Q19</t>
+  </si>
+  <si>
+    <t>Section2-Q17</t>
+  </si>
+  <si>
+    <t>Section3-Q1</t>
+  </si>
+  <si>
+    <t>Section3-Q9</t>
+  </si>
+  <si>
     <t>Section1-Q9</t>
   </si>
   <si>
-    <t>Section2-Q9</t>
-  </si>
-  <si>
-    <t>Section2-Q12</t>
-  </si>
-  <si>
-    <t>Section2-Q3</t>
-  </si>
-  <si>
-    <t>Section3-Q1</t>
+    <t>Section1-Q26</t>
+  </si>
+  <si>
+    <t>Section1-Q7</t>
+  </si>
+  <si>
+    <t>Section2-Q2</t>
+  </si>
+  <si>
+    <t>Section2-Q22</t>
+  </si>
+  <si>
+    <t>Section2-Q4</t>
+  </si>
+  <si>
+    <t>Section3-Q5</t>
+  </si>
+  <si>
+    <t>Section1-Q1</t>
+  </si>
+  <si>
+    <t>Section1-Q28</t>
+  </si>
+  <si>
+    <t>Section1-Q12</t>
+  </si>
+  <si>
+    <t>Section2-Q21</t>
+  </si>
+  <si>
+    <t>Section2-Q5</t>
+  </si>
+  <si>
+    <t>Section2-Q11</t>
+  </si>
+  <si>
+    <t>Section1-Q15</t>
+  </si>
+  <si>
+    <t>Section1-Q17</t>
+  </si>
+  <si>
+    <t>Section2-Q7</t>
+  </si>
+  <si>
+    <t>Section1-Q16</t>
+  </si>
+  <si>
+    <t>Section1-Q21</t>
+  </si>
+  <si>
+    <t>Section1-Q19</t>
+  </si>
+  <si>
+    <t>Section2-Q8</t>
+  </si>
+  <si>
+    <t>Section2-Q23</t>
   </si>
   <si>
     <t>Section3-Q11</t>
   </si>
   <si>
-    <t>Section3-Q7</t>
-  </si>
-  <si>
-    <t>Section1-Q4</t>
-  </si>
-  <si>
-    <t>Section1-Q14</t>
-  </si>
-  <si>
-    <t>Section1-Q5</t>
-  </si>
-  <si>
-    <t>Section2-Q6</t>
-  </si>
-  <si>
-    <t>Section2-Q25</t>
-  </si>
-  <si>
-    <t>Section2-Q13</t>
-  </si>
-  <si>
-    <t>Section3-Q2</t>
+    <t>Section1-Q24</t>
+  </si>
+  <si>
+    <t>Section1-Q23</t>
+  </si>
+  <si>
+    <t>Section2-Q14</t>
+  </si>
+  <si>
+    <t>Section2-Q1</t>
+  </si>
+  <si>
+    <t>Section3-Q12</t>
+  </si>
+  <si>
+    <t>Section1-Q25</t>
+  </si>
+  <si>
+    <t>Section1-Q3</t>
+  </si>
+  <si>
+    <t>Section2-Q15</t>
+  </si>
+  <si>
+    <t>Section3-Q13</t>
+  </si>
+  <si>
+    <t>Roll</t>
+  </si>
+  <si>
+    <t>Section1-Q8</t>
+  </si>
+  <si>
+    <t>Section1-Q18</t>
+  </si>
+  <si>
+    <t>Section1-Q30</t>
+  </si>
+  <si>
+    <t>Section2-Q18</t>
+  </si>
+  <si>
+    <t>Section2-Q20</t>
+  </si>
+  <si>
+    <t>Section2-Q24</t>
+  </si>
+  <si>
+    <t>Section3-Q14</t>
   </si>
   <si>
     <t>Section3-Q15</t>
   </si>
   <si>
-    <t>Section3-Q4</t>
-  </si>
-  <si>
-    <t>Section1-Q13</t>
-  </si>
-  <si>
-    <t>Section1-Q22</t>
-  </si>
-  <si>
-    <t>Section1-Q10</t>
-  </si>
-  <si>
-    <t>Section2-Q10</t>
-  </si>
-  <si>
-    <t>Section2-Q16</t>
-  </si>
-  <si>
-    <t>Section3-Q6</t>
-  </si>
-  <si>
-    <t>Section3-Q10</t>
-  </si>
-  <si>
-    <t>Section3-Q5</t>
-  </si>
-  <si>
-    <t>Section1-Q2</t>
-  </si>
-  <si>
-    <t>Section1-Q29</t>
-  </si>
-  <si>
-    <t>Section1-Q11</t>
-  </si>
-  <si>
-    <t>Section2-Q19</t>
-  </si>
-  <si>
-    <t>Section2-Q17</t>
-  </si>
-  <si>
-    <t>Section3-Q3</t>
-  </si>
-  <si>
-    <t>Section3-Q12</t>
-  </si>
-  <si>
-    <t>Section1-Q1</t>
-  </si>
-  <si>
-    <t>Section1-Q26</t>
-  </si>
-  <si>
-    <t>Section1-Q20</t>
-  </si>
-  <si>
-    <t>Section2-Q2</t>
-  </si>
-  <si>
-    <t>Section2-Q22</t>
-  </si>
-  <si>
-    <t>Section2-Q4</t>
-  </si>
-  <si>
-    <t>Section3-Q13</t>
-  </si>
-  <si>
-    <t>Section3-Q9</t>
-  </si>
-  <si>
-    <t>Section1-Q15</t>
-  </si>
-  <si>
-    <t>Section1-Q28</t>
-  </si>
-  <si>
-    <t>Section1-Q7</t>
-  </si>
-  <si>
-    <t>Section2-Q21</t>
-  </si>
-  <si>
-    <t>Section2-Q5</t>
-  </si>
-  <si>
-    <t>Section2-Q11</t>
-  </si>
-  <si>
-    <t>Section3-Q14</t>
-  </si>
-  <si>
-    <t>Section3-Q8</t>
-  </si>
-  <si>
-    <t>Section1-Q16</t>
-  </si>
-  <si>
-    <t>Section1-Q17</t>
-  </si>
-  <si>
-    <t>Section1-Q12</t>
-  </si>
-  <si>
-    <t>Section2-Q7</t>
-  </si>
-  <si>
-    <t>Section1-Q24</t>
-  </si>
-  <si>
-    <t>Section1-Q21</t>
-  </si>
-  <si>
-    <t>Section2-Q8</t>
-  </si>
-  <si>
-    <t>Section2-Q23</t>
-  </si>
-  <si>
-    <t>Section1-Q25</t>
-  </si>
-  <si>
-    <t>Section1-Q23</t>
-  </si>
-  <si>
-    <t>Section1-Q19</t>
-  </si>
-  <si>
-    <t>Section2-Q14</t>
-  </si>
-  <si>
-    <t>Section2-Q1</t>
-  </si>
-  <si>
-    <t>Section1-Q3</t>
-  </si>
-  <si>
-    <t>Section2-Q15</t>
-  </si>
-  <si>
-    <t>Roll</t>
-  </si>
-  <si>
-    <t>Section1-Q8</t>
-  </si>
-  <si>
-    <t>Section1-Q18</t>
-  </si>
-  <si>
-    <t>Section1-Q30</t>
-  </si>
-  <si>
-    <t>Section2-Q18</t>
-  </si>
-  <si>
-    <t>Section2-Q20</t>
-  </si>
-  <si>
-    <t>Section2-Q24</t>
-  </si>
-  <si>
     <t>934245</t>
   </si>
   <si>
@@ -469,10 +469,10 @@
     <t>C (W)</t>
   </si>
   <si>
+    <t>624690</t>
+  </si>
+  <si>
     <t>B (C)</t>
-  </si>
-  <si>
-    <t>624690</t>
   </si>
   <si>
     <t>C (C)</t>
@@ -533,7 +533,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1138,13 +1138,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q10" zoomScale="110" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+    <sheetView tabSelected="1" zoomScale="53" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:26" ht="15" customHeight="1" thickBot="1">
+    <row r="1" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="15" customHeight="1" thickBot="1">
+    <row r="2" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>757516</v>
       </c>
@@ -1229,18 +1229,18 @@
         <v>24</v>
       </c>
       <c r="C2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E19" si="0">C2*1 + D2*($Z$6)</f>
-        <v>8.5</v>
+        <v>9.75</v>
       </c>
       <c r="F2">
         <f t="shared" ref="F2:F31" si="1">E2/$Y$1*100</f>
-        <v>28.333333333333332</v>
+        <v>32.5</v>
       </c>
       <c r="G2">
         <v>7</v>
@@ -1257,40 +1257,38 @@
         <v>27</v>
       </c>
       <c r="K2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M2">
         <f t="shared" ref="M2:M19" si="4">K2*1 + L2*($Z$6)</f>
-        <v>2.25</v>
+        <v>-0.25</v>
       </c>
       <c r="N2">
         <f t="shared" ref="N2:N31" si="5">M2/$Y$3*100</f>
-        <v>15</v>
+        <v>-1.6666666666666667</v>
       </c>
       <c r="O2">
         <f t="shared" ref="O2:O31" si="6">E2 + I2 + M2</f>
-        <v>17.5</v>
+        <v>16.25</v>
       </c>
       <c r="P2">
         <f t="shared" ref="P2:P31" si="7">O2/$Y$4*100</f>
-        <v>25</v>
+        <v>23.214285714285715</v>
       </c>
       <c r="Q2">
         <f t="shared" ref="Q2:Q31" si="8">_xlfn.RANK.EQ(P2, $P$2:$P$1000, 0)</f>
         <v>2</v>
       </c>
-      <c r="R2" s="10">
-        <v>18</v>
-      </c>
+      <c r="R2" s="10"/>
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
       <c r="U2" s="11"/>
       <c r="V2">
         <f t="shared" ref="V2:V11" si="9">O2+R2+S2+T2+U2</f>
-        <v>35.5</v>
+        <v>16.25</v>
       </c>
       <c r="W2">
         <f t="shared" ref="W2:W31" si="10">_xlfn.RANK.EQ(V2, $V$2:$V$1000, 0)</f>
@@ -1303,7 +1301,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15" customHeight="1" thickBot="1">
+    <row r="3" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>604057</v>
       </c>
@@ -1311,18 +1309,18 @@
         <v>26</v>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>4.5</v>
+        <v>5.75</v>
       </c>
       <c r="F3">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>19.166666666666668</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -1339,18 +1337,18 @@
         <v>-8</v>
       </c>
       <c r="K3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L3">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="M3">
         <f t="shared" si="4"/>
-        <v>2.5</v>
+        <v>1.25</v>
       </c>
       <c r="N3">
         <f t="shared" si="5"/>
-        <v>16.666666666666664</v>
+        <v>8.3333333333333321</v>
       </c>
       <c r="O3">
         <f t="shared" si="6"/>
@@ -1362,21 +1360,19 @@
       </c>
       <c r="Q3">
         <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="R3" s="10">
-        <v>9</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="R3" s="10"/>
       <c r="S3" s="11"/>
       <c r="T3" s="11"/>
       <c r="U3" s="11"/>
       <c r="V3">
         <f t="shared" si="9"/>
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="W3">
         <f t="shared" si="10"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="X3" t="s">
         <v>27</v>
@@ -1385,7 +1381,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15" customHeight="1" thickBot="1">
+    <row r="4" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>934245</v>
       </c>
@@ -1421,40 +1417,38 @@
         <v>3</v>
       </c>
       <c r="K4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M4">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="N4">
         <f t="shared" si="5"/>
-        <v>3.3333333333333335</v>
+        <v>-5</v>
       </c>
       <c r="O4">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0.75</v>
       </c>
       <c r="P4">
         <f t="shared" si="7"/>
-        <v>2.8571428571428572</v>
+        <v>1.0714285714285714</v>
       </c>
       <c r="Q4">
         <f t="shared" si="8"/>
         <v>13</v>
       </c>
-      <c r="R4" s="10">
-        <v>10</v>
-      </c>
+      <c r="R4" s="10"/>
       <c r="S4" s="11"/>
       <c r="T4" s="11"/>
       <c r="U4" s="11"/>
       <c r="V4">
         <f t="shared" si="9"/>
-        <v>12</v>
+        <v>0.75</v>
       </c>
       <c r="W4">
         <f t="shared" si="10"/>
@@ -1465,7 +1459,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" thickBot="1">
+    <row r="5" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>121716</v>
       </c>
@@ -1473,18 +1467,18 @@
         <v>29</v>
       </c>
       <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5">
         <v>6</v>
-      </c>
-      <c r="D5">
-        <v>7</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>4.25</v>
+        <v>5.5</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>14.166666666666666</v>
+        <v>18.333333333333332</v>
       </c>
       <c r="G5">
         <v>3</v>
@@ -1504,44 +1498,42 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M5">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-1.5</v>
       </c>
       <c r="N5">
         <f t="shared" si="5"/>
-        <v>-13.333333333333334</v>
+        <v>-10</v>
       </c>
       <c r="O5">
         <f t="shared" si="6"/>
-        <v>4.75</v>
+        <v>6.5</v>
       </c>
       <c r="P5">
         <f t="shared" si="7"/>
-        <v>6.7857142857142856</v>
+        <v>9.2857142857142865</v>
       </c>
       <c r="Q5">
         <f t="shared" si="8"/>
-        <v>11</v>
-      </c>
-      <c r="R5" s="10">
-        <v>12</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="R5" s="10"/>
       <c r="S5" s="11"/>
       <c r="T5" s="11"/>
       <c r="U5" s="11"/>
       <c r="V5">
         <f t="shared" si="9"/>
-        <v>16.75</v>
+        <v>6.5</v>
       </c>
       <c r="W5">
         <f t="shared" si="10"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1" thickBot="1">
+    <row r="6" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>648081</v>
       </c>
@@ -1594,7 +1586,7 @@
       </c>
       <c r="W6">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Y6" t="s">
         <v>31</v>
@@ -1603,7 +1595,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15" customHeight="1" thickBot="1">
+    <row r="7" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>650004</v>
       </c>
@@ -1656,10 +1648,10 @@
       </c>
       <c r="W7">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="15" customHeight="1" thickBot="1">
+    <row r="8" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>417695</v>
       </c>
@@ -1712,10 +1704,10 @@
       </c>
       <c r="W8">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="15" customHeight="1" thickBot="1">
+    <row r="9" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>400651</v>
       </c>
@@ -1774,24 +1766,22 @@
       </c>
       <c r="Q9">
         <f t="shared" si="8"/>
-        <v>9</v>
-      </c>
-      <c r="R9" s="10">
         <v>10</v>
       </c>
+      <c r="R9" s="10"/>
       <c r="S9" s="11"/>
       <c r="T9" s="11"/>
       <c r="U9" s="11"/>
       <c r="V9">
         <f t="shared" si="9"/>
-        <v>15.5</v>
+        <v>5.5</v>
       </c>
       <c r="W9">
         <f t="shared" si="10"/>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="15" customHeight="1" thickBot="1">
+    <row r="10" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>979212</v>
       </c>
@@ -1827,47 +1817,45 @@
         <v>16</v>
       </c>
       <c r="K10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L10">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M10">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="N10">
         <f t="shared" si="5"/>
-        <v>3.3333333333333335</v>
+        <v>-6.666666666666667</v>
       </c>
       <c r="O10">
         <f t="shared" si="6"/>
-        <v>11.75</v>
+        <v>10.25</v>
       </c>
       <c r="P10">
         <f t="shared" si="7"/>
-        <v>16.785714285714285</v>
+        <v>14.642857142857144</v>
       </c>
       <c r="Q10">
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="R10" s="12">
-        <v>11.5</v>
-      </c>
+      <c r="R10" s="12"/>
       <c r="S10" s="13"/>
       <c r="T10" s="13"/>
       <c r="U10" s="13"/>
       <c r="V10">
         <f t="shared" si="9"/>
-        <v>23.25</v>
+        <v>10.25</v>
       </c>
       <c r="W10">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="15" customHeight="1" thickBot="1">
+    <row r="11" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>542127</v>
       </c>
@@ -1920,10 +1908,10 @@
       </c>
       <c r="W11">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="15" customHeight="1" thickBot="1">
+    <row r="12" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>678535</v>
       </c>
@@ -1972,10 +1960,10 @@
       <c r="U12" s="13"/>
       <c r="W12">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="15" customHeight="1" thickBot="1">
+    <row r="13" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>303558</v>
       </c>
@@ -2028,10 +2016,10 @@
       </c>
       <c r="W13">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="15" customHeight="1" thickBot="1">
+    <row r="14" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>196303</v>
       </c>
@@ -2084,10 +2072,10 @@
       </c>
       <c r="W14">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="15" customHeight="1" thickBot="1">
+    <row r="15" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>146014</v>
       </c>
@@ -2140,10 +2128,10 @@
       </c>
       <c r="W15">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="15" customHeight="1" thickBot="1">
+    <row r="16" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>907183</v>
       </c>
@@ -2196,10 +2184,10 @@
       </c>
       <c r="W16">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="15" customHeight="1" thickBot="1">
+    <row r="17" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>399043</v>
       </c>
@@ -2252,10 +2240,10 @@
       </c>
       <c r="W17">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="15" customHeight="1" thickBot="1">
+    <row r="18" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>643388</v>
       </c>
@@ -2294,44 +2282,42 @@
         <v>0</v>
       </c>
       <c r="L18">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M18">
         <f t="shared" si="4"/>
-        <v>-2.5</v>
+        <v>-2.25</v>
       </c>
       <c r="N18">
         <f t="shared" si="5"/>
-        <v>-16.666666666666664</v>
+        <v>-15</v>
       </c>
       <c r="O18">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>6.25</v>
       </c>
       <c r="P18">
         <f t="shared" si="7"/>
-        <v>8.5714285714285712</v>
+        <v>8.9285714285714288</v>
       </c>
       <c r="Q18">
         <f t="shared" si="8"/>
-        <v>8</v>
-      </c>
-      <c r="R18" s="12">
-        <v>11</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="R18" s="12"/>
       <c r="S18" s="13"/>
       <c r="T18" s="13"/>
       <c r="U18" s="13"/>
       <c r="V18">
         <f t="shared" si="11"/>
-        <v>17</v>
+        <v>6.25</v>
       </c>
       <c r="W18">
         <f t="shared" si="10"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="15" customHeight="1" thickBot="1">
+    <row r="19" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>421527</v>
       </c>
@@ -2392,22 +2378,20 @@
         <f t="shared" si="8"/>
         <v>12</v>
       </c>
-      <c r="R19" s="10">
-        <v>12.5</v>
-      </c>
+      <c r="R19" s="10"/>
       <c r="S19" s="11"/>
       <c r="T19" s="11"/>
       <c r="U19" s="11"/>
       <c r="V19">
         <f t="shared" si="11"/>
-        <v>16</v>
+        <v>3.5</v>
       </c>
       <c r="W19">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="15" customHeight="1" thickBot="1">
+    <row r="20" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>158296</v>
       </c>
@@ -2450,22 +2434,20 @@
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="R20" s="11">
-        <v>7.5</v>
-      </c>
+      <c r="R20" s="11"/>
       <c r="S20" s="11"/>
       <c r="T20" s="11"/>
       <c r="U20" s="11"/>
       <c r="V20">
         <f t="shared" si="11"/>
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="W20">
         <f t="shared" si="10"/>
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="15" customHeight="1" thickBot="1">
+    <row r="21" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>624690</v>
       </c>
@@ -2473,18 +2455,18 @@
         <v>46</v>
       </c>
       <c r="C21">
+        <v>11</v>
+      </c>
+      <c r="D21">
         <v>10</v>
-      </c>
-      <c r="D21">
-        <v>11</v>
       </c>
       <c r="E21">
         <f t="shared" si="12"/>
-        <v>7.25</v>
+        <v>8.5</v>
       </c>
       <c r="F21">
         <f t="shared" si="1"/>
-        <v>24.166666666666668</v>
+        <v>28.333333333333332</v>
       </c>
       <c r="G21">
         <v>3</v>
@@ -2501,47 +2483,45 @@
         <v>12</v>
       </c>
       <c r="K21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L21">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M21">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>-1.5</v>
       </c>
       <c r="N21">
         <f t="shared" si="5"/>
-        <v>6.666666666666667</v>
+        <v>-10</v>
       </c>
       <c r="O21">
         <f t="shared" si="6"/>
-        <v>11.25</v>
+        <v>10</v>
       </c>
       <c r="P21">
         <f t="shared" si="7"/>
-        <v>16.071428571428573</v>
+        <v>14.285714285714285</v>
       </c>
       <c r="Q21">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="R21" s="11">
-        <v>20</v>
-      </c>
+      <c r="R21" s="11"/>
       <c r="S21" s="11"/>
       <c r="T21" s="11"/>
       <c r="U21" s="11"/>
       <c r="V21">
         <f t="shared" si="11"/>
-        <v>31.25</v>
+        <v>10</v>
       </c>
       <c r="W21">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="28.2" customHeight="1" thickBot="1">
+    <row r="22" spans="1:23" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="8">
         <v>575752</v>
       </c>
@@ -2549,18 +2529,18 @@
         <v>47</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D22">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E22">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>2.25</v>
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
-        <v>3.3333333333333335</v>
+        <v>7.5</v>
       </c>
       <c r="G22">
         <v>6</v>
@@ -2580,44 +2560,42 @@
         <v>0</v>
       </c>
       <c r="L22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22">
         <f t="shared" si="14"/>
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="N22">
         <f t="shared" si="5"/>
-        <v>-1.6666666666666667</v>
+        <v>0</v>
       </c>
       <c r="O22">
         <f t="shared" si="6"/>
-        <v>6.75</v>
+        <v>8.25</v>
       </c>
       <c r="P22">
         <f t="shared" si="7"/>
-        <v>9.6428571428571441</v>
+        <v>11.785714285714285</v>
       </c>
       <c r="Q22">
         <f t="shared" si="8"/>
         <v>6</v>
       </c>
-      <c r="R22" s="10">
-        <v>11.5</v>
-      </c>
+      <c r="R22" s="10"/>
       <c r="S22" s="11"/>
       <c r="T22" s="11"/>
       <c r="U22" s="11"/>
       <c r="V22">
         <f t="shared" si="11"/>
-        <v>18.25</v>
+        <v>8.25</v>
       </c>
       <c r="W22">
         <f t="shared" si="10"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="43.8" customHeight="1" thickBot="1">
+    <row r="23" spans="1:23" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="14">
         <v>621172</v>
       </c>
@@ -2625,18 +2603,18 @@
         <v>48</v>
       </c>
       <c r="C23">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D23">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E23">
         <f t="shared" si="12"/>
-        <v>6.25</v>
+        <v>7.5</v>
       </c>
       <c r="F23">
         <f t="shared" si="1"/>
-        <v>20.833333333333336</v>
+        <v>25</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -2668,32 +2646,30 @@
       </c>
       <c r="O23">
         <f t="shared" si="6"/>
-        <v>6.25</v>
+        <v>7.5</v>
       </c>
       <c r="P23">
         <f t="shared" si="7"/>
-        <v>8.9285714285714288</v>
+        <v>10.714285714285714</v>
       </c>
       <c r="Q23">
         <f t="shared" si="8"/>
         <v>7</v>
       </c>
-      <c r="R23" s="10">
-        <v>14.5</v>
-      </c>
+      <c r="R23" s="10"/>
       <c r="S23" s="11"/>
       <c r="T23" s="11"/>
       <c r="U23" s="11"/>
       <c r="V23">
         <f t="shared" si="11"/>
-        <v>20.75</v>
+        <v>7.5</v>
       </c>
       <c r="W23">
         <f t="shared" si="10"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="29.4" customHeight="1" thickBot="1">
+    <row r="24" spans="1:23" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="14">
         <v>764305</v>
       </c>
@@ -2729,47 +2705,45 @@
         <v>24</v>
       </c>
       <c r="K24">
+        <v>2</v>
+      </c>
+      <c r="L24">
         <v>5</v>
-      </c>
-      <c r="L24">
-        <v>4</v>
       </c>
       <c r="M24">
         <f t="shared" si="14"/>
-        <v>4</v>
+        <v>0.75</v>
       </c>
       <c r="N24">
         <f t="shared" si="5"/>
-        <v>26.666666666666668</v>
+        <v>5</v>
       </c>
       <c r="O24">
         <f t="shared" si="6"/>
-        <v>26</v>
+        <v>22.75</v>
       </c>
       <c r="P24">
         <f t="shared" si="7"/>
-        <v>37.142857142857146</v>
+        <v>32.5</v>
       </c>
       <c r="Q24">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="R24" s="10">
-        <v>15.5</v>
-      </c>
+      <c r="R24" s="10"/>
       <c r="S24" s="11"/>
       <c r="T24" s="11"/>
       <c r="U24" s="11"/>
       <c r="V24">
-        <f>O24+R24+S24+T24+U24</f>
-        <v>41.5</v>
+        <f t="shared" si="11"/>
+        <v>22.75</v>
       </c>
       <c r="W24">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="43.8" customHeight="1" thickBot="1">
+    <row r="25" spans="1:23" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="14">
         <v>459889</v>
       </c>
@@ -2777,18 +2751,18 @@
         <v>50</v>
       </c>
       <c r="C25">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E25">
         <f t="shared" si="12"/>
-        <v>10</v>
+        <v>11.25</v>
       </c>
       <c r="F25">
         <f t="shared" si="1"/>
-        <v>33.333333333333329</v>
+        <v>37.5</v>
       </c>
       <c r="G25">
         <v>4</v>
@@ -2820,32 +2794,30 @@
       </c>
       <c r="O25">
         <f t="shared" si="6"/>
-        <v>14</v>
+        <v>15.25</v>
       </c>
       <c r="P25">
         <f t="shared" si="7"/>
-        <v>20</v>
+        <v>21.785714285714285</v>
       </c>
       <c r="Q25">
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="R25" s="10">
-        <v>14</v>
-      </c>
+      <c r="R25" s="10"/>
       <c r="S25" s="11"/>
       <c r="T25" s="11"/>
       <c r="U25" s="11"/>
       <c r="V25">
-        <f>O25+R25+S25+T25+U25</f>
-        <v>28</v>
+        <f t="shared" si="11"/>
+        <v>15.25</v>
       </c>
       <c r="W25">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="15" customHeight="1" thickBot="1">
+    <row r="26" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E26">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -2892,10 +2864,10 @@
       </c>
       <c r="W26">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="15" customHeight="1" thickBot="1">
+    <row r="27" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E27">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -2942,10 +2914,10 @@
       </c>
       <c r="W27">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="15" customHeight="1" thickBot="1">
+    <row r="28" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E28">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -2992,10 +2964,10 @@
       </c>
       <c r="W28">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="15" customHeight="1" thickBot="1">
+    <row r="29" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E29">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -3042,10 +3014,10 @@
       </c>
       <c r="W29">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="15" customHeight="1" thickBot="1">
+    <row r="30" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E30">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -3092,10 +3064,10 @@
       </c>
       <c r="W30">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="15" customHeight="1" thickBot="1">
+    <row r="31" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E31">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -3142,7 +3114,7 @@
       </c>
       <c r="W31">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -3158,7 +3130,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
@@ -3180,7 +3152,7 @@
     <col min="20" max="20" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -3236,7 +3208,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -3253,7 +3225,7 @@
         <v>65</v>
       </c>
       <c r="F2">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H2" t="s">
         <v>66</v>
@@ -3277,13 +3249,13 @@
         <v>69</v>
       </c>
       <c r="P2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q2" t="s">
         <v>70</v>
       </c>
       <c r="R2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S2" t="s">
         <v>71</v>
@@ -3292,7 +3264,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>72</v>
       </c>
@@ -3309,7 +3281,7 @@
         <v>74</v>
       </c>
       <c r="F3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H3" t="s">
         <v>75</v>
@@ -3333,13 +3305,13 @@
         <v>78</v>
       </c>
       <c r="P3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="Q3" t="s">
         <v>79</v>
       </c>
       <c r="R3">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="S3" t="s">
         <v>80</v>
@@ -3348,7 +3320,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>81</v>
       </c>
@@ -3386,39 +3358,39 @@
         <v>4</v>
       </c>
       <c r="O4" t="s">
+        <v>80</v>
+      </c>
+      <c r="P4">
+        <v>2</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>78</v>
+      </c>
+      <c r="R4">
+        <v>6</v>
+      </c>
+      <c r="S4" t="s">
         <v>86</v>
       </c>
-      <c r="P4">
-        <v>5</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="T4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>87</v>
-      </c>
-      <c r="R4">
-        <v>10</v>
-      </c>
-      <c r="S4" t="s">
-        <v>88</v>
-      </c>
-      <c r="T4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
-      <c r="A5" t="s">
-        <v>89</v>
       </c>
       <c r="B5">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D5">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F5">
         <v>6</v>
@@ -3430,219 +3402,219 @@
         <v>3</v>
       </c>
       <c r="J5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K5">
         <v>11</v>
       </c>
       <c r="L5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="M5">
         <v>4</v>
       </c>
       <c r="O5" t="s">
+        <v>92</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>93</v>
+      </c>
+      <c r="R5">
+        <v>6</v>
+      </c>
+      <c r="S5" t="s">
+        <v>92</v>
+      </c>
+      <c r="T5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>94</v>
       </c>
-      <c r="P5">
-        <v>3</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
         <v>95</v>
-      </c>
-      <c r="R5">
-        <v>10</v>
-      </c>
-      <c r="S5" t="s">
-        <v>86</v>
-      </c>
-      <c r="T5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20">
-      <c r="A6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>97</v>
       </c>
       <c r="D6">
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F6">
         <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I6">
         <v>3</v>
       </c>
       <c r="J6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K6">
         <v>11</v>
       </c>
       <c r="L6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="M6">
         <v>4</v>
       </c>
       <c r="O6" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="P6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="R6">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="S6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="T6">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D7">
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I7">
         <v>3</v>
       </c>
       <c r="J7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K7">
         <v>11</v>
       </c>
       <c r="L7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="M7">
         <v>3</v>
       </c>
       <c r="O7" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="P7">
         <v>1</v>
       </c>
       <c r="Q7" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="R7">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="S7" t="s">
-        <v>111</v>
+        <v>69</v>
       </c>
       <c r="T7">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D8">
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="F8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I8">
         <v>3</v>
       </c>
       <c r="J8" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="K8">
         <v>11</v>
       </c>
       <c r="L8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="M8">
         <v>3</v>
       </c>
       <c r="O8" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="P8">
         <v>1</v>
       </c>
       <c r="Q8" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="R8">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="S8" t="s">
+        <v>93</v>
+      </c>
+      <c r="T8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>110</v>
-      </c>
-      <c r="T8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20">
-      <c r="A9" t="s">
-        <v>116</v>
       </c>
       <c r="B9">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D9">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="F9">
         <v>4</v>
@@ -3654,63 +3626,63 @@
         <v>2</v>
       </c>
       <c r="J9" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="K9">
         <v>11</v>
       </c>
       <c r="L9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="M9">
         <v>3</v>
       </c>
       <c r="O9" t="s">
+        <v>115</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>71</v>
+      </c>
+      <c r="R9">
+        <v>2</v>
+      </c>
+      <c r="S9" t="s">
         <v>79</v>
       </c>
-      <c r="P9">
-        <v>1</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>94</v>
-      </c>
-      <c r="R9">
-        <v>6</v>
-      </c>
-      <c r="S9" t="s">
-        <v>78</v>
-      </c>
       <c r="T9">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B10">
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D10">
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>122</v>
+        <v>63</v>
       </c>
       <c r="F10">
         <v>4</v>
       </c>
       <c r="H10" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I10">
         <v>2</v>
       </c>
       <c r="J10" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="K10">
         <v>10</v>
@@ -3722,78 +3694,78 @@
         <v>3</v>
       </c>
       <c r="O10" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>80</v>
+      </c>
+      <c r="R10">
         <v>1</v>
       </c>
-      <c r="Q10" t="s">
-        <v>103</v>
-      </c>
-      <c r="R10">
-        <v>6</v>
-      </c>
       <c r="S10" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="T10">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D11">
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="F11">
         <v>4</v>
       </c>
       <c r="H11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I11">
         <v>2</v>
       </c>
       <c r="J11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="K11">
         <v>10</v>
       </c>
       <c r="L11" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="M11">
         <v>2</v>
       </c>
       <c r="O11" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>69</v>
+      </c>
+      <c r="R11">
         <v>1</v>
       </c>
-      <c r="Q11" t="s">
-        <v>88</v>
-      </c>
-      <c r="R11">
-        <v>5</v>
-      </c>
       <c r="S11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="T11">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3812,7 +3784,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="10" width="13" customWidth="1"/>
@@ -3823,45 +3795,45 @@
     <col min="66" max="71" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71">
+    <row r="1" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>72</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="G1" s="15" t="s">
         <v>63</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="K1" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="L1" s="15" t="s">
-        <v>91</v>
-      </c>
       <c r="M1" s="15" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="N1" s="15" t="s">
         <v>81</v>
@@ -3870,76 +3842,76 @@
         <v>73</v>
       </c>
       <c r="P1" s="15" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="Q1" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="R1" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="S1" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="T1" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="R1" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="S1" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="T1" s="15" t="s">
-        <v>122</v>
-      </c>
       <c r="U1" s="15" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="W1" s="15" t="s">
         <v>82</v>
       </c>
       <c r="X1" s="15" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="Y1" s="15" t="s">
         <v>116</v>
       </c>
       <c r="Z1" s="15" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AA1" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AB1" s="15" t="s">
         <v>64</v>
       </c>
       <c r="AC1" s="15" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="AD1" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AE1" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="AF1" s="15" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="AG1" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AH1" s="15" t="s">
         <v>68</v>
       </c>
       <c r="AI1" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AJ1" s="15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="AK1" s="15" t="s">
         <v>75</v>
       </c>
       <c r="AL1" s="15" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="AM1" s="15" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="AN1" s="15" t="s">
         <v>66</v>
@@ -3948,7 +3920,7 @@
         <v>84</v>
       </c>
       <c r="AP1" s="15" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="AQ1" s="15" t="s">
         <v>67</v>
@@ -3957,88 +3929,88 @@
         <v>77</v>
       </c>
       <c r="AS1" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="AT1" s="15" t="s">
         <v>123</v>
-      </c>
-      <c r="AT1" s="15" t="s">
-        <v>126</v>
       </c>
       <c r="AU1" s="15" t="s">
         <v>85</v>
       </c>
       <c r="AV1" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AW1" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="AX1" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="AY1" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ1" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="BA1" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="BB1" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="BC1" s="15" t="s">
         <v>131</v>
-      </c>
-      <c r="AX1" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AY1" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="AZ1" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="BA1" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="BB1" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="BC1" s="15" t="s">
-        <v>133</v>
       </c>
       <c r="BD1" s="15" t="s">
         <v>76</v>
       </c>
       <c r="BE1" s="15" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="BF1" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="BG1" s="15" t="s">
         <v>78</v>
-      </c>
-      <c r="BG1" s="15" t="s">
-        <v>94</v>
       </c>
       <c r="BH1" s="15" t="s">
         <v>80</v>
       </c>
       <c r="BI1" s="15" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="BJ1" s="15" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="BK1" s="15" t="s">
         <v>71</v>
       </c>
       <c r="BL1" s="15" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="BM1" s="15" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="BN1" s="15" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="BO1" s="15" t="s">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="BP1" s="15" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="BQ1" s="15" t="s">
-        <v>102</v>
+        <v>124</v>
       </c>
       <c r="BR1" s="15" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
       <c r="BS1" s="15" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:71">
+    <row r="2" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>134</v>
       </c>
@@ -4207,8 +4179,8 @@
       <c r="BD2" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BE2" s="18" t="s">
-        <v>144</v>
+      <c r="BE2" s="17" t="s">
+        <v>140</v>
       </c>
       <c r="BF2" s="17" t="s">
         <v>141</v>
@@ -4237,28 +4209,18 @@
       <c r="BN2" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="BO2" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BP2" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BQ2" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BR2" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BS2" s="16" t="s">
-        <v>136</v>
-      </c>
+      <c r="BO2" s="16"/>
+      <c r="BP2" s="16"/>
+      <c r="BQ2" s="16"/>
+      <c r="BR2" s="16"/>
+      <c r="BS2" s="16"/>
     </row>
-    <row r="3" spans="1:71">
+    <row r="3" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>145</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>144</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>135</v>
@@ -4281,8 +4243,8 @@
       <c r="I3" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="J3" s="17" t="s">
-        <v>140</v>
+      <c r="J3" s="18" t="s">
+        <v>145</v>
       </c>
       <c r="K3" s="18" t="s">
         <v>142</v>
@@ -4330,7 +4292,7 @@
         <v>139</v>
       </c>
       <c r="Z3" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AA3" s="17" t="s">
         <v>140</v>
@@ -4351,7 +4313,7 @@
         <v>136</v>
       </c>
       <c r="AG3" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AH3" s="16" t="s">
         <v>136</v>
@@ -4422,11 +4384,11 @@
       <c r="BD3" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BE3" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="BF3" s="18" t="s">
-        <v>137</v>
+      <c r="BE3" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="BF3" s="17" t="s">
+        <v>135</v>
       </c>
       <c r="BG3" s="16" t="s">
         <v>136</v>
@@ -4452,23 +4414,13 @@
       <c r="BN3" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BO3" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BP3" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BQ3" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BR3" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BS3" s="16" t="s">
-        <v>136</v>
-      </c>
+      <c r="BO3" s="16"/>
+      <c r="BP3" s="16"/>
+      <c r="BQ3" s="16"/>
+      <c r="BR3" s="16"/>
+      <c r="BS3" s="16"/>
     </row>
-    <row r="4" spans="1:71">
+    <row r="4" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>147</v>
       </c>
@@ -4476,7 +4428,7 @@
         <v>136</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>136</v>
@@ -4496,8 +4448,8 @@
       <c r="I4" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="J4" s="17" t="s">
-        <v>140</v>
+      <c r="J4" s="18" t="s">
+        <v>145</v>
       </c>
       <c r="K4" s="18" t="s">
         <v>142</v>
@@ -4667,28 +4619,18 @@
       <c r="BN4" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BO4" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BP4" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BQ4" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BR4" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BS4" s="16" t="s">
-        <v>136</v>
-      </c>
+      <c r="BO4" s="16"/>
+      <c r="BP4" s="16"/>
+      <c r="BQ4" s="16"/>
+      <c r="BR4" s="16"/>
+      <c r="BS4" s="16"/>
     </row>
-    <row r="5" spans="1:71">
+    <row r="5" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>149</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>141</v>
@@ -4760,7 +4702,7 @@
         <v>135</v>
       </c>
       <c r="Z5" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AA5" s="17" t="s">
         <v>143</v>
@@ -4778,7 +4720,7 @@
         <v>136</v>
       </c>
       <c r="AF5" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AG5" s="17" t="s">
         <v>135</v>
@@ -4852,11 +4794,11 @@
       <c r="BD5" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BE5" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="BF5" s="18" t="s">
-        <v>137</v>
+      <c r="BE5" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="BF5" s="17" t="s">
+        <v>135</v>
       </c>
       <c r="BG5" s="18" t="s">
         <v>139</v>
@@ -4882,23 +4824,13 @@
       <c r="BN5" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BO5" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BP5" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BQ5" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BR5" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BS5" s="16" t="s">
-        <v>136</v>
-      </c>
+      <c r="BO5" s="16"/>
+      <c r="BP5" s="16"/>
+      <c r="BQ5" s="16"/>
+      <c r="BR5" s="16"/>
+      <c r="BS5" s="16"/>
     </row>
-    <row r="6" spans="1:71">
+    <row r="6" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>151</v>
       </c>
@@ -4926,8 +4858,8 @@
       <c r="I6" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="J6" s="17" t="s">
-        <v>140</v>
+      <c r="J6" s="18" t="s">
+        <v>145</v>
       </c>
       <c r="K6" s="17" t="s">
         <v>141</v>
@@ -4975,7 +4907,7 @@
         <v>143</v>
       </c>
       <c r="Z6" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AA6" s="17" t="s">
         <v>140</v>
@@ -4996,7 +4928,7 @@
         <v>136</v>
       </c>
       <c r="AG6" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AH6" s="17" t="s">
         <v>138</v>
@@ -5097,23 +5029,13 @@
       <c r="BN6" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BO6" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BP6" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="BQ6" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BR6" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BS6" s="16" t="s">
-        <v>136</v>
-      </c>
+      <c r="BO6" s="16"/>
+      <c r="BP6" s="16"/>
+      <c r="BQ6" s="16"/>
+      <c r="BR6" s="16"/>
+      <c r="BS6" s="16"/>
     </row>
-    <row r="7" spans="1:71">
+    <row r="7" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>152</v>
       </c>
@@ -5121,7 +5043,7 @@
         <v>138</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>146</v>
@@ -5141,8 +5063,8 @@
       <c r="I7" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="J7" s="17" t="s">
-        <v>140</v>
+      <c r="J7" s="18" t="s">
+        <v>145</v>
       </c>
       <c r="K7" s="17" t="s">
         <v>140</v>
@@ -5282,8 +5204,8 @@
       <c r="BD7" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="BE7" s="18" t="s">
-        <v>144</v>
+      <c r="BE7" s="17" t="s">
+        <v>140</v>
       </c>
       <c r="BF7" s="17" t="s">
         <v>141</v>
@@ -5298,7 +5220,7 @@
         <v>141</v>
       </c>
       <c r="BJ7" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="BK7" s="17" t="s">
         <v>140</v>
@@ -5312,23 +5234,13 @@
       <c r="BN7" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="BO7" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="BP7" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="BQ7" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="BR7" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="BS7" s="18" t="s">
-        <v>146</v>
-      </c>
+      <c r="BO7" s="16"/>
+      <c r="BP7" s="16"/>
+      <c r="BQ7" s="16"/>
+      <c r="BR7" s="16"/>
+      <c r="BS7" s="16"/>
     </row>
-    <row r="8" spans="1:71">
+    <row r="8" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>153</v>
       </c>
@@ -5336,7 +5248,7 @@
         <v>135</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>146</v>
@@ -5405,7 +5317,7 @@
         <v>143</v>
       </c>
       <c r="Z8" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AA8" s="18" t="s">
         <v>142</v>
@@ -5527,28 +5439,18 @@
       <c r="BN8" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BO8" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BP8" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BQ8" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BR8" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BS8" s="16" t="s">
-        <v>136</v>
-      </c>
+      <c r="BO8" s="16"/>
+      <c r="BP8" s="16"/>
+      <c r="BQ8" s="16"/>
+      <c r="BR8" s="16"/>
+      <c r="BS8" s="16"/>
     </row>
-    <row r="9" spans="1:71">
+    <row r="9" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>156</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>136</v>
@@ -5742,31 +5644,21 @@
       <c r="BN9" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BO9" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BP9" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BQ9" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BR9" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BS9" s="16" t="s">
-        <v>136</v>
-      </c>
+      <c r="BO9" s="16"/>
+      <c r="BP9" s="16"/>
+      <c r="BQ9" s="16"/>
+      <c r="BR9" s="16"/>
+      <c r="BS9" s="16"/>
     </row>
-    <row r="10" spans="1:71">
+    <row r="10" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
         <v>157</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>136</v>
@@ -5775,7 +5667,7 @@
         <v>137</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G10" s="18" t="s">
         <v>146</v>
@@ -5786,8 +5678,8 @@
       <c r="I10" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="J10" s="17" t="s">
-        <v>140</v>
+      <c r="J10" s="18" t="s">
+        <v>145</v>
       </c>
       <c r="K10" s="16" t="s">
         <v>136</v>
@@ -5895,7 +5787,7 @@
         <v>139</v>
       </c>
       <c r="AT10" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AU10" s="16" t="s">
         <v>136</v>
@@ -5904,7 +5796,7 @@
         <v>139</v>
       </c>
       <c r="AW10" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AX10" s="16" t="s">
         <v>136</v>
@@ -5927,11 +5819,11 @@
       <c r="BD10" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BE10" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="BF10" s="18" t="s">
-        <v>137</v>
+      <c r="BE10" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="BF10" s="17" t="s">
+        <v>135</v>
       </c>
       <c r="BG10" s="17" t="s">
         <v>138</v>
@@ -5943,7 +5835,7 @@
         <v>136</v>
       </c>
       <c r="BJ10" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="BK10" s="17" t="s">
         <v>135</v>
@@ -5957,31 +5849,21 @@
       <c r="BN10" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BO10" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BP10" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BQ10" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BR10" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BS10" s="16" t="s">
-        <v>136</v>
-      </c>
+      <c r="BO10" s="16"/>
+      <c r="BP10" s="16"/>
+      <c r="BQ10" s="16"/>
+      <c r="BR10" s="16"/>
+      <c r="BS10" s="16"/>
     </row>
-    <row r="11" spans="1:71">
+    <row r="11" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>158</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>146</v>
@@ -5990,7 +5872,7 @@
         <v>137</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G11" s="18" t="s">
         <v>146</v>
@@ -6001,14 +5883,14 @@
       <c r="I11" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="J11" s="17" t="s">
-        <v>140</v>
+      <c r="J11" s="18" t="s">
+        <v>145</v>
       </c>
       <c r="K11" s="17" t="s">
         <v>140</v>
       </c>
       <c r="L11" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M11" s="18" t="s">
         <v>146</v>
@@ -6158,7 +6040,7 @@
         <v>136</v>
       </c>
       <c r="BJ11" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="BK11" s="17" t="s">
         <v>135</v>
@@ -6172,23 +6054,13 @@
       <c r="BN11" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="BO11" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BP11" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BQ11" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BR11" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BS11" s="16" t="s">
-        <v>136</v>
-      </c>
+      <c r="BO11" s="16"/>
+      <c r="BP11" s="16"/>
+      <c r="BQ11" s="16"/>
+      <c r="BR11" s="16"/>
+      <c r="BS11" s="16"/>
     </row>
-    <row r="12" spans="1:71">
+    <row r="12" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
         <v>159</v>
       </c>
@@ -6196,7 +6068,7 @@
         <v>135</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>136</v>
@@ -6223,7 +6095,7 @@
         <v>136</v>
       </c>
       <c r="L12" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M12" s="16" t="s">
         <v>136</v>
@@ -6387,28 +6259,18 @@
       <c r="BN12" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BO12" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="BP12" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BQ12" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BR12" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BS12" s="16" t="s">
-        <v>136</v>
-      </c>
+      <c r="BO12" s="16"/>
+      <c r="BP12" s="16"/>
+      <c r="BQ12" s="16"/>
+      <c r="BR12" s="16"/>
+      <c r="BS12" s="16"/>
     </row>
-    <row r="13" spans="1:71">
+    <row r="13" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
         <v>161</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>136</v>
@@ -6431,14 +6293,14 @@
       <c r="I13" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="J13" s="17" t="s">
-        <v>140</v>
+      <c r="J13" s="18" t="s">
+        <v>145</v>
       </c>
       <c r="K13" s="16" t="s">
         <v>136</v>
       </c>
       <c r="L13" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M13" s="17" t="s">
         <v>138</v>
@@ -6602,23 +6464,13 @@
       <c r="BN13" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BO13" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BP13" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BQ13" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="BR13" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="BS13" s="16" t="s">
-        <v>136</v>
-      </c>
+      <c r="BO13" s="16"/>
+      <c r="BP13" s="16"/>
+      <c r="BQ13" s="16"/>
+      <c r="BR13" s="16"/>
+      <c r="BS13" s="16"/>
     </row>
-    <row r="14" spans="1:71">
+    <row r="14" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>162</v>
       </c>
@@ -6626,7 +6478,7 @@
         <v>136</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D14" s="16" t="s">
         <v>136</v>
@@ -6695,7 +6547,7 @@
         <v>139</v>
       </c>
       <c r="Z14" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AA14" s="16" t="s">
         <v>136</v>
@@ -6764,7 +6616,7 @@
         <v>136</v>
       </c>
       <c r="AW14" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AX14" s="16" t="s">
         <v>136</v>
@@ -6787,11 +6639,11 @@
       <c r="BD14" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BE14" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="BF14" s="18" t="s">
-        <v>137</v>
+      <c r="BE14" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="BF14" s="17" t="s">
+        <v>135</v>
       </c>
       <c r="BG14" s="17" t="s">
         <v>138</v>
@@ -6803,7 +6655,7 @@
         <v>143</v>
       </c>
       <c r="BJ14" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="BK14" s="17" t="s">
         <v>135</v>
@@ -6817,23 +6669,13 @@
       <c r="BN14" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BO14" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BP14" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="BQ14" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="BR14" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="BS14" s="17" t="s">
-        <v>141</v>
-      </c>
+      <c r="BO14" s="16"/>
+      <c r="BP14" s="16"/>
+      <c r="BQ14" s="16"/>
+      <c r="BR14" s="16"/>
+      <c r="BS14" s="16"/>
     </row>
-    <row r="15" spans="1:71">
+    <row r="15" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>163</v>
       </c>
@@ -6841,7 +6683,7 @@
         <v>135</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D15" s="16" t="s">
         <v>136</v>
@@ -6868,7 +6710,7 @@
         <v>135</v>
       </c>
       <c r="L15" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M15" s="18" t="s">
         <v>146</v>
@@ -6910,7 +6752,7 @@
         <v>139</v>
       </c>
       <c r="Z15" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AA15" s="18" t="s">
         <v>142</v>
@@ -6922,7 +6764,7 @@
         <v>136</v>
       </c>
       <c r="AD15" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AE15" s="18" t="s">
         <v>137</v>
@@ -6931,7 +6773,7 @@
         <v>136</v>
       </c>
       <c r="AG15" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AH15" s="18" t="s">
         <v>146</v>
@@ -6970,7 +6812,7 @@
         <v>136</v>
       </c>
       <c r="AT15" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AU15" s="18" t="s">
         <v>142</v>
@@ -7002,11 +6844,11 @@
       <c r="BD15" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BE15" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="BF15" s="18" t="s">
-        <v>137</v>
+      <c r="BE15" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="BF15" s="17" t="s">
+        <v>135</v>
       </c>
       <c r="BG15" s="18" t="s">
         <v>139</v>
@@ -7018,7 +6860,7 @@
         <v>143</v>
       </c>
       <c r="BJ15" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="BK15" s="17" t="s">
         <v>135</v>
@@ -7032,21 +6874,11 @@
       <c r="BN15" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BO15" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BP15" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BQ15" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="BR15" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="BS15" s="16" t="s">
-        <v>136</v>
-      </c>
+      <c r="BO15" s="16"/>
+      <c r="BP15" s="16"/>
+      <c r="BQ15" s="16"/>
+      <c r="BR15" s="16"/>
+      <c r="BS15" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update Mock 1 data and recalculate thresholds
Processed updated Mock 1.xlsx file and recalculated thresholds based on new student performance data. New thresholds: Section 1: 5.50 marks, Section 2: 1.00 marks, Section 3: 0.25 marks. Updated all JSON data files with the latest results.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Results/Mock 1.xlsx
+++ b/Results/Mock 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\results giver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55BD355-5465-4E2A-B789-CC6A47586B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F881116-1BAF-4C57-B427-8327023314DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="164">
   <si>
     <t>ID</t>
   </si>
@@ -244,120 +244,135 @@
     <t>Section2-Q3</t>
   </si>
   <si>
+    <t>Section3-Q4</t>
+  </si>
+  <si>
+    <t>Section3-Q11</t>
+  </si>
+  <si>
     <t>Section3-Q6</t>
   </si>
   <si>
+    <t>Section1-Q4</t>
+  </si>
+  <si>
+    <t>Section1-Q14</t>
+  </si>
+  <si>
+    <t>Section1-Q10</t>
+  </si>
+  <si>
+    <t>Section2-Q6</t>
+  </si>
+  <si>
+    <t>Section2-Q25</t>
+  </si>
+  <si>
+    <t>Section2-Q13</t>
+  </si>
+  <si>
+    <t>Section3-Q2</t>
+  </si>
+  <si>
+    <t>Section3-Q15</t>
+  </si>
+  <si>
+    <t>Section3-Q7</t>
+  </si>
+  <si>
+    <t>Section1-Q13</t>
+  </si>
+  <si>
+    <t>Section1-Q22</t>
+  </si>
+  <si>
+    <t>Section1-Q11</t>
+  </si>
+  <si>
+    <t>Section2-Q10</t>
+  </si>
+  <si>
+    <t>Section2-Q16</t>
+  </si>
+  <si>
+    <t>Section3-Q9</t>
+  </si>
+  <si>
     <t>Section3-Q10</t>
   </si>
   <si>
-    <t>Section3-Q7</t>
-  </si>
-  <si>
-    <t>Section1-Q4</t>
-  </si>
-  <si>
-    <t>Section1-Q14</t>
-  </si>
-  <si>
-    <t>Section1-Q10</t>
-  </si>
-  <si>
-    <t>Section2-Q6</t>
-  </si>
-  <si>
-    <t>Section2-Q25</t>
-  </si>
-  <si>
-    <t>Section2-Q13</t>
+    <t>Section3-Q5</t>
+  </si>
+  <si>
+    <t>Section1-Q2</t>
+  </si>
+  <si>
+    <t>Section1-Q29</t>
+  </si>
+  <si>
+    <t>Section1-Q20</t>
+  </si>
+  <si>
+    <t>Section2-Q19</t>
+  </si>
+  <si>
+    <t>Section2-Q17</t>
+  </si>
+  <si>
+    <t>Section3-Q1</t>
+  </si>
+  <si>
+    <t>Section3-Q12</t>
+  </si>
+  <si>
+    <t>Section1-Q9</t>
+  </si>
+  <si>
+    <t>Section1-Q26</t>
+  </si>
+  <si>
+    <t>Section1-Q7</t>
+  </si>
+  <si>
+    <t>Section2-Q2</t>
+  </si>
+  <si>
+    <t>Section2-Q22</t>
+  </si>
+  <si>
+    <t>Section2-Q4</t>
+  </si>
+  <si>
+    <t>Section3-Q13</t>
   </si>
   <si>
     <t>Section3-Q3</t>
   </si>
   <si>
+    <t>Section1-Q1</t>
+  </si>
+  <si>
+    <t>Section1-Q28</t>
+  </si>
+  <si>
+    <t>Section1-Q12</t>
+  </si>
+  <si>
+    <t>Section2-Q21</t>
+  </si>
+  <si>
+    <t>Section2-Q5</t>
+  </si>
+  <si>
+    <t>Section2-Q11</t>
+  </si>
+  <si>
+    <t>Section3-Q14</t>
+  </si>
+  <si>
     <t>Section3-Q8</t>
   </si>
   <si>
-    <t>Section3-Q4</t>
-  </si>
-  <si>
-    <t>Section1-Q13</t>
-  </si>
-  <si>
-    <t>Section1-Q22</t>
-  </si>
-  <si>
-    <t>Section1-Q11</t>
-  </si>
-  <si>
-    <t>Section2-Q10</t>
-  </si>
-  <si>
-    <t>Section2-Q16</t>
-  </si>
-  <si>
-    <t>Section3-Q2</t>
-  </si>
-  <si>
-    <t>Section1-Q2</t>
-  </si>
-  <si>
-    <t>Section1-Q29</t>
-  </si>
-  <si>
-    <t>Section1-Q20</t>
-  </si>
-  <si>
-    <t>Section2-Q19</t>
-  </si>
-  <si>
-    <t>Section2-Q17</t>
-  </si>
-  <si>
-    <t>Section3-Q1</t>
-  </si>
-  <si>
-    <t>Section3-Q9</t>
-  </si>
-  <si>
-    <t>Section1-Q9</t>
-  </si>
-  <si>
-    <t>Section1-Q26</t>
-  </si>
-  <si>
-    <t>Section1-Q7</t>
-  </si>
-  <si>
-    <t>Section2-Q2</t>
-  </si>
-  <si>
-    <t>Section2-Q22</t>
-  </si>
-  <si>
-    <t>Section2-Q4</t>
-  </si>
-  <si>
-    <t>Section3-Q5</t>
-  </si>
-  <si>
-    <t>Section1-Q1</t>
-  </si>
-  <si>
-    <t>Section1-Q28</t>
-  </si>
-  <si>
-    <t>Section1-Q12</t>
-  </si>
-  <si>
-    <t>Section2-Q21</t>
-  </si>
-  <si>
-    <t>Section2-Q5</t>
-  </si>
-  <si>
-    <t>Section2-Q11</t>
-  </si>
-  <si>
     <t>Section1-Q15</t>
   </si>
   <si>
@@ -382,9 +397,6 @@
     <t>Section2-Q23</t>
   </si>
   <si>
-    <t>Section3-Q11</t>
-  </si>
-  <si>
     <t>Section1-Q24</t>
   </si>
   <si>
@@ -397,9 +409,6 @@
     <t>Section2-Q1</t>
   </si>
   <si>
-    <t>Section3-Q12</t>
-  </si>
-  <si>
     <t>Section1-Q25</t>
   </si>
   <si>
@@ -409,9 +418,6 @@
     <t>Section2-Q15</t>
   </si>
   <si>
-    <t>Section3-Q13</t>
-  </si>
-  <si>
     <t>Roll</t>
   </si>
   <si>
@@ -431,12 +437,6 @@
   </si>
   <si>
     <t>Section2-Q24</t>
-  </si>
-  <si>
-    <t>Section3-Q14</t>
-  </si>
-  <si>
-    <t>Section3-Q15</t>
   </si>
   <si>
     <t>934245</t>
@@ -533,7 +533,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1138,13 +1138,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="53" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A2" s="1">
         <v>757516</v>
       </c>
@@ -1257,26 +1257,26 @@
         <v>27</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M2">
         <f t="shared" ref="M2:M19" si="4">K2*1 + L2*($Z$6)</f>
-        <v>-0.25</v>
+        <v>1</v>
       </c>
       <c r="N2">
         <f t="shared" ref="N2:N31" si="5">M2/$Y$3*100</f>
-        <v>-1.6666666666666667</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="O2">
         <f t="shared" ref="O2:O31" si="6">E2 + I2 + M2</f>
-        <v>16.25</v>
+        <v>17.5</v>
       </c>
       <c r="P2">
         <f t="shared" ref="P2:P31" si="7">O2/$Y$4*100</f>
-        <v>23.214285714285715</v>
+        <v>25</v>
       </c>
       <c r="Q2">
         <f t="shared" ref="Q2:Q31" si="8">_xlfn.RANK.EQ(P2, $P$2:$P$1000, 0)</f>
@@ -1288,7 +1288,7 @@
       <c r="U2" s="11"/>
       <c r="V2">
         <f t="shared" ref="V2:V11" si="9">O2+R2+S2+T2+U2</f>
-        <v>16.25</v>
+        <v>17.5</v>
       </c>
       <c r="W2">
         <f t="shared" ref="W2:W31" si="10">_xlfn.RANK.EQ(V2, $V$2:$V$1000, 0)</f>
@@ -1301,7 +1301,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A3" s="1">
         <v>604057</v>
       </c>
@@ -1337,10 +1337,10 @@
         <v>-8</v>
       </c>
       <c r="K3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L3">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="M3">
         <f t="shared" si="4"/>
@@ -1360,7 +1360,7 @@
       </c>
       <c r="Q3">
         <f t="shared" si="8"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R3" s="10"/>
       <c r="S3" s="11"/>
@@ -1372,7 +1372,7 @@
       </c>
       <c r="W3">
         <f t="shared" si="10"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="X3" t="s">
         <v>27</v>
@@ -1381,7 +1381,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A4" s="1">
         <v>934245</v>
       </c>
@@ -1417,30 +1417,30 @@
         <v>3</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M4">
         <f t="shared" si="4"/>
-        <v>-0.75</v>
+        <v>-2</v>
       </c>
       <c r="N4">
         <f t="shared" si="5"/>
-        <v>-5</v>
+        <v>-13.333333333333334</v>
       </c>
       <c r="O4">
         <f t="shared" si="6"/>
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="P4">
         <f t="shared" si="7"/>
-        <v>1.0714285714285714</v>
+        <v>-0.7142857142857143</v>
       </c>
       <c r="Q4">
         <f t="shared" si="8"/>
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="R4" s="10"/>
       <c r="S4" s="11"/>
@@ -1448,18 +1448,18 @@
       <c r="U4" s="11"/>
       <c r="V4">
         <f t="shared" si="9"/>
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="W4">
         <f t="shared" si="10"/>
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="Y4">
         <f>SUM(Y1:Y3)</f>
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A5" s="1">
         <v>121716</v>
       </c>
@@ -1495,30 +1495,30 @@
         <v>10</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L5">
         <v>6</v>
       </c>
       <c r="M5">
         <f t="shared" si="4"/>
-        <v>-1.5</v>
+        <v>0.5</v>
       </c>
       <c r="N5">
         <f t="shared" si="5"/>
-        <v>-10</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="O5">
         <f t="shared" si="6"/>
-        <v>6.5</v>
+        <v>8.5</v>
       </c>
       <c r="P5">
         <f t="shared" si="7"/>
-        <v>9.2857142857142865</v>
+        <v>12.142857142857142</v>
       </c>
       <c r="Q5">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R5" s="10"/>
       <c r="S5" s="11"/>
@@ -1526,14 +1526,14 @@
       <c r="U5" s="11"/>
       <c r="V5">
         <f t="shared" si="9"/>
-        <v>6.5</v>
+        <v>8.5</v>
       </c>
       <c r="W5">
         <f t="shared" si="10"/>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A6" s="1">
         <v>648081</v>
       </c>
@@ -1574,7 +1574,7 @@
       </c>
       <c r="Q6">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R6" s="10"/>
       <c r="S6" s="11"/>
@@ -1586,7 +1586,7 @@
       </c>
       <c r="W6">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Y6" t="s">
         <v>31</v>
@@ -1595,7 +1595,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A7" s="1">
         <v>650004</v>
       </c>
@@ -1636,7 +1636,7 @@
       </c>
       <c r="Q7">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R7" s="10"/>
       <c r="S7" s="11"/>
@@ -1648,10 +1648,10 @@
       </c>
       <c r="W7">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A8" s="1">
         <v>417695</v>
       </c>
@@ -1692,7 +1692,7 @@
       </c>
       <c r="Q8">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R8" s="12"/>
       <c r="S8" s="13"/>
@@ -1704,10 +1704,10 @@
       </c>
       <c r="W8">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A9" s="1">
         <v>400651</v>
       </c>
@@ -1743,30 +1743,30 @@
         <v>4</v>
       </c>
       <c r="K9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M9">
         <f t="shared" si="4"/>
-        <v>0.25</v>
+        <v>-1</v>
       </c>
       <c r="N9">
         <f t="shared" si="5"/>
-        <v>1.6666666666666667</v>
+        <v>-6.666666666666667</v>
       </c>
       <c r="O9">
         <f t="shared" si="6"/>
-        <v>5.5</v>
+        <v>4.25</v>
       </c>
       <c r="P9">
         <f t="shared" si="7"/>
-        <v>7.8571428571428568</v>
+        <v>6.0714285714285712</v>
       </c>
       <c r="Q9">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R9" s="10"/>
       <c r="S9" s="11"/>
@@ -1774,14 +1774,14 @@
       <c r="U9" s="11"/>
       <c r="V9">
         <f t="shared" si="9"/>
-        <v>5.5</v>
+        <v>4.25</v>
       </c>
       <c r="W9">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A10" s="1">
         <v>979212</v>
       </c>
@@ -1817,30 +1817,30 @@
         <v>16</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L10">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M10">
         <f t="shared" si="4"/>
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="N10">
         <f t="shared" si="5"/>
-        <v>-6.666666666666667</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="O10">
         <f t="shared" si="6"/>
-        <v>10.25</v>
+        <v>11.75</v>
       </c>
       <c r="P10">
         <f t="shared" si="7"/>
-        <v>14.642857142857144</v>
+        <v>16.785714285714285</v>
       </c>
       <c r="Q10">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R10" s="12"/>
       <c r="S10" s="13"/>
@@ -1848,14 +1848,14 @@
       <c r="U10" s="13"/>
       <c r="V10">
         <f t="shared" si="9"/>
-        <v>10.25</v>
+        <v>11.75</v>
       </c>
       <c r="W10">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A11" s="1">
         <v>542127</v>
       </c>
@@ -1896,7 +1896,7 @@
       </c>
       <c r="Q11">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R11" s="10"/>
       <c r="S11" s="11"/>
@@ -1908,10 +1908,10 @@
       </c>
       <c r="W11">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A12" s="1">
         <v>678535</v>
       </c>
@@ -1952,7 +1952,7 @@
       </c>
       <c r="Q12">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R12" s="12"/>
       <c r="S12" s="13"/>
@@ -1960,10 +1960,10 @@
       <c r="U12" s="13"/>
       <c r="W12">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A13" s="1">
         <v>303558</v>
       </c>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="Q13">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R13" s="12"/>
       <c r="S13" s="13"/>
@@ -2016,10 +2016,10 @@
       </c>
       <c r="W13">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A14" s="1">
         <v>196303</v>
       </c>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="Q14">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R14" s="12"/>
       <c r="S14" s="13"/>
@@ -2072,10 +2072,10 @@
       </c>
       <c r="W14">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A15" s="1">
         <v>146014</v>
       </c>
@@ -2116,7 +2116,7 @@
       </c>
       <c r="Q15">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R15" s="10"/>
       <c r="S15" s="11"/>
@@ -2128,10 +2128,10 @@
       </c>
       <c r="W15">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A16" s="1">
         <v>907183</v>
       </c>
@@ -2172,7 +2172,7 @@
       </c>
       <c r="Q16">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R16" s="10"/>
       <c r="S16" s="11"/>
@@ -2184,10 +2184,10 @@
       </c>
       <c r="W16">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" ht="15" customHeight="1" thickBot="1">
       <c r="A17" s="1">
         <v>399043</v>
       </c>
@@ -2228,7 +2228,7 @@
       </c>
       <c r="Q17">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R17" s="10"/>
       <c r="S17" s="11"/>
@@ -2240,10 +2240,10 @@
       </c>
       <c r="W17">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23" ht="15" customHeight="1" thickBot="1">
       <c r="A18" s="1">
         <v>643388</v>
       </c>
@@ -2279,30 +2279,30 @@
         <v>4</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L18">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="M18">
         <f t="shared" si="4"/>
-        <v>-2.25</v>
+        <v>2.5</v>
       </c>
       <c r="N18">
         <f t="shared" si="5"/>
-        <v>-15</v>
+        <v>16.666666666666664</v>
       </c>
       <c r="O18">
         <f t="shared" si="6"/>
-        <v>6.25</v>
+        <v>11</v>
       </c>
       <c r="P18">
         <f t="shared" si="7"/>
-        <v>8.9285714285714288</v>
+        <v>15.714285714285714</v>
       </c>
       <c r="Q18">
         <f t="shared" si="8"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="R18" s="12"/>
       <c r="S18" s="13"/>
@@ -2310,14 +2310,14 @@
       <c r="U18" s="13"/>
       <c r="V18">
         <f t="shared" si="11"/>
-        <v>6.25</v>
+        <v>11</v>
       </c>
       <c r="W18">
         <f t="shared" si="10"/>
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" ht="15" customHeight="1" thickBot="1">
       <c r="A19" s="1">
         <v>421527</v>
       </c>
@@ -2353,26 +2353,26 @@
         <v>8</v>
       </c>
       <c r="K19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L19">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M19">
         <f t="shared" si="4"/>
-        <v>1.5</v>
+        <v>0.25</v>
       </c>
       <c r="N19">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="O19">
         <f t="shared" si="6"/>
-        <v>3.5</v>
+        <v>2.25</v>
       </c>
       <c r="P19">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>3.214285714285714</v>
       </c>
       <c r="Q19">
         <f t="shared" si="8"/>
@@ -2384,14 +2384,14 @@
       <c r="U19" s="11"/>
       <c r="V19">
         <f t="shared" si="11"/>
-        <v>3.5</v>
+        <v>2.25</v>
       </c>
       <c r="W19">
         <f t="shared" si="10"/>
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" ht="15" customHeight="1" thickBot="1">
       <c r="A20" s="5">
         <v>158296</v>
       </c>
@@ -2432,7 +2432,7 @@
       </c>
       <c r="Q20">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R20" s="11"/>
       <c r="S20" s="11"/>
@@ -2444,10 +2444,10 @@
       </c>
       <c r="W20">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" ht="15" customHeight="1" thickBot="1">
       <c r="A21" s="5">
         <v>624690</v>
       </c>
@@ -2483,30 +2483,30 @@
         <v>12</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L21">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M21">
         <f t="shared" si="14"/>
-        <v>-1.5</v>
+        <v>1</v>
       </c>
       <c r="N21">
         <f t="shared" si="5"/>
-        <v>-10</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="O21">
         <f t="shared" si="6"/>
-        <v>10</v>
+        <v>12.5</v>
       </c>
       <c r="P21">
         <f t="shared" si="7"/>
-        <v>14.285714285714285</v>
+        <v>17.857142857142858</v>
       </c>
       <c r="Q21">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R21" s="11"/>
       <c r="S21" s="11"/>
@@ -2514,14 +2514,14 @@
       <c r="U21" s="11"/>
       <c r="V21">
         <f t="shared" si="11"/>
-        <v>10</v>
+        <v>12.5</v>
       </c>
       <c r="W21">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" ht="28.2" customHeight="1" thickBot="1">
       <c r="A22" s="8">
         <v>575752</v>
       </c>
@@ -2560,27 +2560,27 @@
         <v>0</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M22">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="N22">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-1.6666666666666667</v>
       </c>
       <c r="O22">
         <f t="shared" si="6"/>
-        <v>8.25</v>
+        <v>8</v>
       </c>
       <c r="P22">
         <f t="shared" si="7"/>
-        <v>11.785714285714285</v>
+        <v>11.428571428571429</v>
       </c>
       <c r="Q22">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="R22" s="10"/>
       <c r="S22" s="11"/>
@@ -2588,14 +2588,14 @@
       <c r="U22" s="11"/>
       <c r="V22">
         <f t="shared" si="11"/>
-        <v>8.25</v>
+        <v>8</v>
       </c>
       <c r="W22">
         <f t="shared" si="10"/>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" ht="43.8" customHeight="1" thickBot="1">
       <c r="A23" s="14">
         <v>621172</v>
       </c>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="Q23">
         <f t="shared" si="8"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="R23" s="10"/>
       <c r="S23" s="11"/>
@@ -2666,10 +2666,10 @@
       </c>
       <c r="W23">
         <f t="shared" si="10"/>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" ht="29.4" customHeight="1" thickBot="1">
       <c r="A24" s="14">
         <v>764305</v>
       </c>
@@ -2705,26 +2705,26 @@
         <v>24</v>
       </c>
       <c r="K24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M24">
         <f t="shared" si="14"/>
-        <v>0.75</v>
+        <v>1.5</v>
       </c>
       <c r="N24">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="O24">
         <f t="shared" si="6"/>
-        <v>22.75</v>
+        <v>23.5</v>
       </c>
       <c r="P24">
         <f t="shared" si="7"/>
-        <v>32.5</v>
+        <v>33.571428571428569</v>
       </c>
       <c r="Q24">
         <f t="shared" si="8"/>
@@ -2736,14 +2736,14 @@
       <c r="U24" s="11"/>
       <c r="V24">
         <f t="shared" si="11"/>
-        <v>22.75</v>
+        <v>23.5</v>
       </c>
       <c r="W24">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" ht="43.8" customHeight="1" thickBot="1">
       <c r="A25" s="14">
         <v>459889</v>
       </c>
@@ -2779,26 +2779,26 @@
         <v>16</v>
       </c>
       <c r="K25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M25">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="N25">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>8.3333333333333321</v>
       </c>
       <c r="O25">
         <f t="shared" si="6"/>
-        <v>15.25</v>
+        <v>16.5</v>
       </c>
       <c r="P25">
         <f t="shared" si="7"/>
-        <v>21.785714285714285</v>
+        <v>23.571428571428569</v>
       </c>
       <c r="Q25">
         <f t="shared" si="8"/>
@@ -2810,14 +2810,14 @@
       <c r="U25" s="11"/>
       <c r="V25">
         <f t="shared" si="11"/>
-        <v>15.25</v>
+        <v>16.5</v>
       </c>
       <c r="W25">
         <f t="shared" si="10"/>
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" ht="15" customHeight="1" thickBot="1">
       <c r="E26">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -2852,7 +2852,7 @@
       </c>
       <c r="Q26">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R26" s="10"/>
       <c r="S26" s="11"/>
@@ -2864,10 +2864,10 @@
       </c>
       <c r="W26">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" ht="15" customHeight="1" thickBot="1">
       <c r="E27">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -2902,7 +2902,7 @@
       </c>
       <c r="Q27">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R27" s="10"/>
       <c r="S27" s="11"/>
@@ -2914,10 +2914,10 @@
       </c>
       <c r="W27">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" ht="15" customHeight="1" thickBot="1">
       <c r="E28">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -2952,7 +2952,7 @@
       </c>
       <c r="Q28">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R28" s="10"/>
       <c r="S28" s="11"/>
@@ -2964,10 +2964,10 @@
       </c>
       <c r="W28">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" ht="15" customHeight="1" thickBot="1">
       <c r="E29">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -3002,7 +3002,7 @@
       </c>
       <c r="Q29">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R29" s="12"/>
       <c r="S29" s="13"/>
@@ -3014,10 +3014,10 @@
       </c>
       <c r="W29">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" ht="15" customHeight="1" thickBot="1">
       <c r="E30">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -3052,7 +3052,7 @@
       </c>
       <c r="Q30">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R30" s="10"/>
       <c r="S30" s="11"/>
@@ -3064,10 +3064,10 @@
       </c>
       <c r="W30">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" ht="15" customHeight="1" thickBot="1">
       <c r="E31">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -3102,7 +3102,7 @@
       </c>
       <c r="Q31">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R31" s="12"/>
       <c r="S31" s="13"/>
@@ -3114,7 +3114,7 @@
       </c>
       <c r="W31">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -3130,7 +3130,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
@@ -3152,7 +3152,7 @@
     <col min="20" max="20" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -3249,22 +3249,22 @@
         <v>69</v>
       </c>
       <c r="P2">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="Q2" t="s">
         <v>70</v>
       </c>
       <c r="R2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S2" t="s">
         <v>71</v>
       </c>
       <c r="T2">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
         <v>72</v>
       </c>
@@ -3305,22 +3305,22 @@
         <v>78</v>
       </c>
       <c r="P3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q3" t="s">
         <v>79</v>
       </c>
       <c r="R3">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="S3" t="s">
         <v>80</v>
       </c>
       <c r="T3">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
         <v>81</v>
       </c>
@@ -3358,39 +3358,39 @@
         <v>4</v>
       </c>
       <c r="O4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="P4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q4" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="R4">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="S4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="T4">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B5">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D5">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F5">
         <v>6</v>
@@ -3402,69 +3402,69 @@
         <v>3</v>
       </c>
       <c r="J5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="K5">
         <v>11</v>
       </c>
       <c r="L5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="M5">
         <v>4</v>
       </c>
       <c r="O5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="P5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="R5">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="S5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="T5">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B6">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D6">
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F6">
         <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I6">
         <v>3</v>
       </c>
       <c r="J6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="K6">
         <v>11</v>
       </c>
       <c r="L6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="M6">
         <v>4</v>
@@ -3473,148 +3473,148 @@
         <v>70</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q6" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="R6">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="S6" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="T6">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D7">
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F7">
         <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="I7">
         <v>3</v>
       </c>
       <c r="J7" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="K7">
         <v>11</v>
       </c>
       <c r="L7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="M7">
         <v>3</v>
       </c>
       <c r="O7" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="P7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q7" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="R7">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="S7" t="s">
-        <v>69</v>
+        <v>111</v>
       </c>
       <c r="T7">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B8">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="D8">
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F8">
         <v>4</v>
       </c>
       <c r="H8" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I8">
         <v>3</v>
       </c>
       <c r="J8" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="K8">
         <v>11</v>
       </c>
       <c r="L8" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="M8">
         <v>3</v>
       </c>
       <c r="O8" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="P8">
         <v>1</v>
       </c>
       <c r="Q8" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="R8">
+        <v>7</v>
+      </c>
+      <c r="S8" t="s">
+        <v>78</v>
+      </c>
+      <c r="T8">
         <v>4</v>
       </c>
-      <c r="S8" t="s">
-        <v>93</v>
-      </c>
-      <c r="T8">
-        <v>6</v>
-      </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B9">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D9">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="F9">
         <v>4</v>
@@ -3626,45 +3626,45 @@
         <v>2</v>
       </c>
       <c r="J9" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="K9">
         <v>11</v>
       </c>
       <c r="L9" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M9">
         <v>3</v>
       </c>
       <c r="O9" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="P9">
         <v>0</v>
       </c>
       <c r="Q9" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="R9">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="S9" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="T9">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B10">
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D10">
         <v>8</v>
@@ -3676,13 +3676,13 @@
         <v>4</v>
       </c>
       <c r="H10" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="I10">
         <v>2</v>
       </c>
       <c r="J10" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="K10">
         <v>10</v>
@@ -3694,78 +3694,78 @@
         <v>3</v>
       </c>
       <c r="O10" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="P10">
         <v>0</v>
       </c>
       <c r="Q10" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="R10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="S10" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="T10">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B11">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D11">
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F11">
         <v>4</v>
       </c>
       <c r="H11" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="I11">
         <v>2</v>
       </c>
       <c r="J11" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="K11">
         <v>10</v>
       </c>
       <c r="L11" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="M11">
         <v>2</v>
       </c>
       <c r="O11" t="s">
-        <v>124</v>
+        <v>79</v>
       </c>
       <c r="P11">
         <v>0</v>
       </c>
       <c r="Q11" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="R11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S11" t="s">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="T11">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -3778,13 +3778,13 @@
   <dimension ref="A1:BS15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BG2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="BO13" sqref="BO13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="10" width="13" customWidth="1"/>
@@ -3795,18 +3795,18 @@
     <col min="66" max="71" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:71">
       <c r="A1" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>125</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>122</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>72</v>
@@ -3818,13 +3818,13 @@
         <v>63</v>
       </c>
       <c r="H1" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="J1" s="15" t="s">
         <v>96</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>94</v>
       </c>
       <c r="K1" s="15" t="s">
         <v>74</v>
@@ -3833,7 +3833,7 @@
         <v>83</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="N1" s="15" t="s">
         <v>81</v>
@@ -3842,76 +3842,76 @@
         <v>73</v>
       </c>
       <c r="P1" s="15" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="Q1" s="15" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="R1" s="15" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="T1" s="15" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="U1" s="15" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="W1" s="15" t="s">
         <v>82</v>
       </c>
       <c r="X1" s="15" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="Y1" s="15" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="Z1" s="15" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AA1" s="15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AB1" s="15" t="s">
         <v>64</v>
       </c>
       <c r="AC1" s="15" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="AD1" s="15" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="AE1" s="15" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AF1" s="15" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="AG1" s="15" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="AH1" s="15" t="s">
         <v>68</v>
       </c>
       <c r="AI1" s="15" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AJ1" s="15" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="AK1" s="15" t="s">
         <v>75</v>
       </c>
       <c r="AL1" s="15" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="AM1" s="15" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="AN1" s="15" t="s">
         <v>66</v>
@@ -3920,7 +3920,7 @@
         <v>84</v>
       </c>
       <c r="AP1" s="15" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="AQ1" s="15" t="s">
         <v>67</v>
@@ -3929,88 +3929,88 @@
         <v>77</v>
       </c>
       <c r="AS1" s="15" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="AT1" s="15" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AU1" s="15" t="s">
         <v>85</v>
       </c>
       <c r="AV1" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AW1" s="15" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AX1" s="15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AY1" s="15" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AZ1" s="15" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="BA1" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="BB1" s="15" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="BC1" s="15" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="BD1" s="15" t="s">
         <v>76</v>
       </c>
       <c r="BE1" s="15" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="BF1" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="BG1" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="BH1" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="BI1" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="BJ1" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="BK1" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="BL1" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="BM1" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="BG1" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="BH1" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="BI1" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="BJ1" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="BK1" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="BL1" s="15" t="s">
+      <c r="BN1" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="BO1" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="BP1" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="BQ1" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="BR1" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="BS1" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="BM1" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="BN1" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="BO1" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="BP1" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="BQ1" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="BR1" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="BS1" s="15" t="s">
-        <v>133</v>
-      </c>
     </row>
-    <row r="2" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:71">
       <c r="A2" s="16" t="s">
         <v>134</v>
       </c>
@@ -4206,16 +4206,26 @@
       <c r="BM2" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="BN2" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="BO2" s="16"/>
-      <c r="BP2" s="16"/>
-      <c r="BQ2" s="16"/>
-      <c r="BR2" s="16"/>
-      <c r="BS2" s="16"/>
+      <c r="BN2" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="BO2" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BP2" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BQ2" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BR2" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BS2" s="16" t="s">
+        <v>136</v>
+      </c>
     </row>
-    <row r="3" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:71">
       <c r="A3" s="16" t="s">
         <v>144</v>
       </c>
@@ -4387,14 +4397,14 @@
       <c r="BE3" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="BF3" s="17" t="s">
-        <v>135</v>
+      <c r="BF3" s="18" t="s">
+        <v>137</v>
       </c>
       <c r="BG3" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BH3" s="17" t="s">
-        <v>140</v>
+      <c r="BH3" s="18" t="s">
+        <v>145</v>
       </c>
       <c r="BI3" s="17" t="s">
         <v>143</v>
@@ -4414,13 +4424,23 @@
       <c r="BN3" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BO3" s="16"/>
-      <c r="BP3" s="16"/>
-      <c r="BQ3" s="16"/>
-      <c r="BR3" s="16"/>
-      <c r="BS3" s="16"/>
+      <c r="BO3" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BP3" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BQ3" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BR3" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BS3" s="16" t="s">
+        <v>136</v>
+      </c>
     </row>
-    <row r="4" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:71">
       <c r="A4" s="16" t="s">
         <v>147</v>
       </c>
@@ -4589,8 +4609,8 @@
       <c r="BD4" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BE4" s="17" t="s">
-        <v>135</v>
+      <c r="BE4" s="18" t="s">
+        <v>137</v>
       </c>
       <c r="BF4" s="17" t="s">
         <v>138</v>
@@ -4598,8 +4618,8 @@
       <c r="BG4" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BH4" s="18" t="s">
-        <v>146</v>
+      <c r="BH4" s="17" t="s">
+        <v>143</v>
       </c>
       <c r="BI4" s="16" t="s">
         <v>136</v>
@@ -4619,13 +4639,23 @@
       <c r="BN4" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BO4" s="16"/>
-      <c r="BP4" s="16"/>
-      <c r="BQ4" s="16"/>
-      <c r="BR4" s="16"/>
-      <c r="BS4" s="16"/>
+      <c r="BO4" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BP4" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BQ4" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BR4" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BS4" s="16" t="s">
+        <v>136</v>
+      </c>
     </row>
-    <row r="5" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:71">
       <c r="A5" s="16" t="s">
         <v>149</v>
       </c>
@@ -4794,17 +4824,17 @@
       <c r="BD5" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BE5" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="BF5" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="BG5" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="BH5" s="17" t="s">
-        <v>140</v>
+      <c r="BE5" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="BF5" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="BG5" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="BH5" s="18" t="s">
+        <v>145</v>
       </c>
       <c r="BI5" s="17" t="s">
         <v>143</v>
@@ -4818,19 +4848,29 @@
       <c r="BL5" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="BM5" s="18" t="s">
-        <v>139</v>
+      <c r="BM5" s="17" t="s">
+        <v>141</v>
       </c>
       <c r="BN5" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BO5" s="16"/>
-      <c r="BP5" s="16"/>
-      <c r="BQ5" s="16"/>
-      <c r="BR5" s="16"/>
-      <c r="BS5" s="16"/>
+      <c r="BO5" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BP5" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BQ5" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BR5" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BS5" s="16" t="s">
+        <v>136</v>
+      </c>
     </row>
-    <row r="6" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:71">
       <c r="A6" s="16" t="s">
         <v>151</v>
       </c>
@@ -5029,13 +5069,23 @@
       <c r="BN6" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BO6" s="16"/>
-      <c r="BP6" s="16"/>
-      <c r="BQ6" s="16"/>
-      <c r="BR6" s="16"/>
-      <c r="BS6" s="16"/>
+      <c r="BO6" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BP6" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="BQ6" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BR6" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BS6" s="16" t="s">
+        <v>136</v>
+      </c>
     </row>
-    <row r="7" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:71">
       <c r="A7" s="16" t="s">
         <v>152</v>
       </c>
@@ -5210,37 +5260,47 @@
       <c r="BF7" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="BG7" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="BH7" s="17" t="s">
-        <v>140</v>
+      <c r="BG7" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="BH7" s="18" t="s">
+        <v>145</v>
       </c>
       <c r="BI7" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="BJ7" s="18" t="s">
-        <v>145</v>
+      <c r="BJ7" s="17" t="s">
+        <v>140</v>
       </c>
       <c r="BK7" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="BL7" s="18" t="s">
+      <c r="BL7" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="BM7" s="18" t="s">
         <v>146</v>
-      </c>
-      <c r="BM7" s="17" t="s">
-        <v>143</v>
       </c>
       <c r="BN7" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="BO7" s="16"/>
-      <c r="BP7" s="16"/>
-      <c r="BQ7" s="16"/>
-      <c r="BR7" s="16"/>
-      <c r="BS7" s="16"/>
+      <c r="BO7" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="BP7" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="BQ7" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="BR7" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="BS7" s="17" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="8" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:71">
       <c r="A8" s="16" t="s">
         <v>153</v>
       </c>
@@ -5439,13 +5499,23 @@
       <c r="BN8" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BO8" s="16"/>
-      <c r="BP8" s="16"/>
-      <c r="BQ8" s="16"/>
-      <c r="BR8" s="16"/>
-      <c r="BS8" s="16"/>
+      <c r="BO8" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BP8" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BQ8" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BR8" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BS8" s="16" t="s">
+        <v>136</v>
+      </c>
     </row>
-    <row r="9" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:71">
       <c r="A9" s="16" t="s">
         <v>156</v>
       </c>
@@ -5623,8 +5693,8 @@
       <c r="BG9" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BH9" s="18" t="s">
-        <v>146</v>
+      <c r="BH9" s="17" t="s">
+        <v>143</v>
       </c>
       <c r="BI9" s="17" t="s">
         <v>143</v>
@@ -5644,13 +5714,23 @@
       <c r="BN9" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BO9" s="16"/>
-      <c r="BP9" s="16"/>
-      <c r="BQ9" s="16"/>
-      <c r="BR9" s="16"/>
-      <c r="BS9" s="16"/>
+      <c r="BO9" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BP9" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BQ9" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BR9" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BS9" s="16" t="s">
+        <v>136</v>
+      </c>
     </row>
-    <row r="10" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:71">
       <c r="A10" s="16" t="s">
         <v>157</v>
       </c>
@@ -5822,20 +5902,20 @@
       <c r="BE10" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="BF10" s="17" t="s">
-        <v>135</v>
+      <c r="BF10" s="18" t="s">
+        <v>137</v>
       </c>
       <c r="BG10" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="BH10" s="17" t="s">
+      <c r="BH10" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="BI10" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BJ10" s="17" t="s">
         <v>140</v>
-      </c>
-      <c r="BI10" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BJ10" s="18" t="s">
-        <v>145</v>
       </c>
       <c r="BK10" s="17" t="s">
         <v>135</v>
@@ -5849,13 +5929,23 @@
       <c r="BN10" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BO10" s="16"/>
-      <c r="BP10" s="16"/>
-      <c r="BQ10" s="16"/>
-      <c r="BR10" s="16"/>
-      <c r="BS10" s="16"/>
+      <c r="BO10" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BP10" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BQ10" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BR10" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BS10" s="16" t="s">
+        <v>136</v>
+      </c>
     </row>
-    <row r="11" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:71">
       <c r="A11" s="16" t="s">
         <v>158</v>
       </c>
@@ -6033,14 +6123,14 @@
       <c r="BG11" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BH11" s="17" t="s">
+      <c r="BH11" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="BI11" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BJ11" s="17" t="s">
         <v>140</v>
-      </c>
-      <c r="BI11" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BJ11" s="18" t="s">
-        <v>145</v>
       </c>
       <c r="BK11" s="17" t="s">
         <v>135</v>
@@ -6048,19 +6138,29 @@
       <c r="BL11" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BM11" s="17" t="s">
-        <v>143</v>
+      <c r="BM11" s="18" t="s">
+        <v>146</v>
       </c>
       <c r="BN11" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="BO11" s="16"/>
-      <c r="BP11" s="16"/>
-      <c r="BQ11" s="16"/>
-      <c r="BR11" s="16"/>
-      <c r="BS11" s="16"/>
+      <c r="BO11" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BP11" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BQ11" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BR11" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BS11" s="16" t="s">
+        <v>136</v>
+      </c>
     </row>
-    <row r="12" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:71">
       <c r="A12" s="16" t="s">
         <v>159</v>
       </c>
@@ -6229,8 +6329,8 @@
       <c r="BD12" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BE12" s="17" t="s">
-        <v>135</v>
+      <c r="BE12" s="18" t="s">
+        <v>137</v>
       </c>
       <c r="BF12" s="17" t="s">
         <v>138</v>
@@ -6238,8 +6338,8 @@
       <c r="BG12" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="BH12" s="17" t="s">
-        <v>140</v>
+      <c r="BH12" s="18" t="s">
+        <v>145</v>
       </c>
       <c r="BI12" s="17" t="s">
         <v>143</v>
@@ -6253,19 +6353,29 @@
       <c r="BL12" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="BM12" s="17" t="s">
-        <v>143</v>
+      <c r="BM12" s="18" t="s">
+        <v>146</v>
       </c>
       <c r="BN12" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BO12" s="16"/>
-      <c r="BP12" s="16"/>
-      <c r="BQ12" s="16"/>
-      <c r="BR12" s="16"/>
-      <c r="BS12" s="16"/>
+      <c r="BO12" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="BP12" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BQ12" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BR12" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BS12" s="16" t="s">
+        <v>136</v>
+      </c>
     </row>
-    <row r="13" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:71">
       <c r="A13" s="16" t="s">
         <v>161</v>
       </c>
@@ -6443,8 +6553,8 @@
       <c r="BG13" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BH13" s="17" t="s">
-        <v>140</v>
+      <c r="BH13" s="18" t="s">
+        <v>145</v>
       </c>
       <c r="BI13" s="17" t="s">
         <v>143</v>
@@ -6464,13 +6574,23 @@
       <c r="BN13" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BO13" s="16"/>
-      <c r="BP13" s="16"/>
-      <c r="BQ13" s="16"/>
-      <c r="BR13" s="16"/>
-      <c r="BS13" s="16"/>
+      <c r="BO13" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BP13" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BQ13" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="BR13" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="BS13" s="16" t="s">
+        <v>136</v>
+      </c>
     </row>
-    <row r="14" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:71">
       <c r="A14" s="16" t="s">
         <v>162</v>
       </c>
@@ -6642,20 +6762,20 @@
       <c r="BE14" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="BF14" s="17" t="s">
-        <v>135</v>
+      <c r="BF14" s="18" t="s">
+        <v>137</v>
       </c>
       <c r="BG14" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="BH14" s="17" t="s">
-        <v>140</v>
+      <c r="BH14" s="18" t="s">
+        <v>145</v>
       </c>
       <c r="BI14" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="BJ14" s="18" t="s">
-        <v>145</v>
+      <c r="BJ14" s="17" t="s">
+        <v>140</v>
       </c>
       <c r="BK14" s="17" t="s">
         <v>135</v>
@@ -6663,19 +6783,29 @@
       <c r="BL14" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="BM14" s="17" t="s">
+      <c r="BM14" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="BN14" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BO14" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BP14" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="BQ14" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="BR14" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="BN14" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="BO14" s="16"/>
-      <c r="BP14" s="16"/>
-      <c r="BQ14" s="16"/>
-      <c r="BR14" s="16"/>
-      <c r="BS14" s="16"/>
+      <c r="BS14" s="17" t="s">
+        <v>141</v>
+      </c>
     </row>
-    <row r="15" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:71">
       <c r="A15" s="16" t="s">
         <v>163</v>
       </c>
@@ -6847,20 +6977,20 @@
       <c r="BE15" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="BF15" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="BG15" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="BH15" s="17" t="s">
-        <v>140</v>
+      <c r="BF15" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="BG15" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="BH15" s="18" t="s">
+        <v>145</v>
       </c>
       <c r="BI15" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="BJ15" s="18" t="s">
-        <v>145</v>
+      <c r="BJ15" s="17" t="s">
+        <v>140</v>
       </c>
       <c r="BK15" s="17" t="s">
         <v>135</v>
@@ -6874,11 +7004,21 @@
       <c r="BN15" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="BO15" s="16"/>
-      <c r="BP15" s="16"/>
-      <c r="BQ15" s="16"/>
-      <c r="BR15" s="16"/>
-      <c r="BS15" s="16"/>
+      <c r="BO15" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BP15" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BQ15" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="BR15" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="BS15" s="16" t="s">
+        <v>136</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>